<commit_message>
List of parts updated
</commit_message>
<xml_diff>
--- a/Documentation/List of parts.xlsx
+++ b/Documentation/List of parts.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\GitHub\S-car-lett-A1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\GitHub\S-car-lett-A1\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB8AD4A2-FB31-4AEB-AA2B-05C4BFB6D509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A6ED6F-5A60-43FB-A6CA-FB1930E22BFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="173">
   <si>
     <t>STATUS</t>
   </si>
@@ -543,6 +543,18 @@
   </si>
   <si>
     <t>YX-X801 battery deep discharge protector (12 V DC, 10 A)</t>
+  </si>
+  <si>
+    <t>Raspberry Pi Pico W</t>
+  </si>
+  <si>
+    <t>https://allegro.pl/oferta/raspberry-pi-pico-w-12351876204</t>
+  </si>
+  <si>
+    <t>https://allegro.pl/oferta/obudowa-raspberry-pi-pico-transparentna-13052332067</t>
+  </si>
+  <si>
+    <t>Raspberry Pi Pico W enclosure (transparent)</t>
   </si>
 </sst>
 </file>
@@ -553,7 +565,7 @@
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$zł-415]_-;\-* #,##0.00\ [$zł-415]_-;_-* &quot;-&quot;??\ [$zł-415]_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;zł&quot;"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -572,6 +584,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -644,8 +662,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AB844FC7-134C-46AA-BA3E-7A1662AFAC66}" name="Main" displayName="Main" ref="A1:H73" totalsRowShown="0">
-  <autoFilter ref="A1:H73" xr:uid="{AB844FC7-134C-46AA-BA3E-7A1662AFAC66}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AB844FC7-134C-46AA-BA3E-7A1662AFAC66}" name="Main" displayName="Main" ref="A1:H75" totalsRowShown="0">
+  <autoFilter ref="A1:H75" xr:uid="{AB844FC7-134C-46AA-BA3E-7A1662AFAC66}"/>
   <tableColumns count="8">
     <tableColumn id="2" xr3:uid="{D7367AC1-33ED-4746-B20F-DF2A97AAD7C1}" name="PART NAME"/>
     <tableColumn id="7" xr3:uid="{A49DEDCB-A3F3-4E47-A1CB-9507B06E98EF}" name="QTY."/>
@@ -937,10 +955,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J73"/>
+  <dimension ref="A1:J75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H74" sqref="H74"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H76" sqref="H76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1014,7 +1032,7 @@
       </c>
       <c r="J2" s="1">
         <f>SUM(Main[PRICE (ALL PCS.)])</f>
-        <v>1789.1199999999997</v>
+        <v>1830.6299999999997</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1517,7 +1535,7 @@
         <v>1.57</v>
       </c>
       <c r="E21" s="4">
-        <f t="shared" ref="E21:E26" si="1">PRODUCT(B21*D21)</f>
+        <f t="shared" ref="E21:E25" si="1">PRODUCT(B21*D21)</f>
         <v>4.71</v>
       </c>
       <c r="F21" s="2">
@@ -1639,8 +1657,8 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
-        <v>50</v>
+      <c r="A26" t="s">
+        <v>172</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -1649,25 +1667,25 @@
         <v>10</v>
       </c>
       <c r="D26" s="4">
-        <v>4</v>
+        <v>6.9</v>
       </c>
       <c r="E26" s="4">
-        <f t="shared" si="1"/>
-        <v>4</v>
+        <f t="shared" ref="E26" si="2">PRODUCT(B26*D26)</f>
+        <v>6.9</v>
       </c>
       <c r="F26" s="2">
         <v>45181</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>76</v>
+        <v>171</v>
       </c>
       <c r="H26" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>66</v>
+      <c r="A27" s="5" t="s">
+        <v>50</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -1676,17 +1694,17 @@
         <v>10</v>
       </c>
       <c r="D27" s="4">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E27" s="4">
-        <f t="shared" ref="E27:E30" si="2">PRODUCT(B27*D27)</f>
-        <v>20</v>
+        <f>PRODUCT(B27*D27)</f>
+        <v>4</v>
       </c>
       <c r="F27" s="2">
         <v>45181</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H27" t="s">
         <v>69</v>
@@ -1694,7 +1712,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -1703,17 +1721,17 @@
         <v>10</v>
       </c>
       <c r="D28" s="4">
-        <v>15.5</v>
+        <v>20</v>
       </c>
       <c r="E28" s="4">
-        <f t="shared" si="2"/>
-        <v>15.5</v>
+        <f t="shared" ref="E28:E31" si="3">PRODUCT(B28*D28)</f>
+        <v>20</v>
       </c>
       <c r="F28" s="2">
         <v>45181</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H28" t="s">
         <v>69</v>
@@ -1721,7 +1739,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -1733,14 +1751,14 @@
         <v>15.5</v>
       </c>
       <c r="E29" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15.5</v>
       </c>
       <c r="F29" s="2">
         <v>45181</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H29" t="s">
         <v>69</v>
@@ -1748,7 +1766,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -1757,17 +1775,17 @@
         <v>10</v>
       </c>
       <c r="D30" s="4">
-        <v>12</v>
+        <v>15.5</v>
       </c>
       <c r="E30" s="4">
-        <f t="shared" si="2"/>
-        <v>12</v>
+        <f t="shared" si="3"/>
+        <v>15.5</v>
       </c>
       <c r="F30" s="2">
         <v>45181</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H30" t="s">
         <v>69</v>
@@ -1775,26 +1793,26 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>148</v>
+        <v>71</v>
       </c>
       <c r="B31">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C31" t="s">
         <v>10</v>
       </c>
       <c r="D31" s="4">
-        <v>1.5</v>
+        <v>12</v>
       </c>
       <c r="E31" s="4">
-        <f t="shared" ref="E31:E32" si="3">PRODUCT(B31*D31)</f>
-        <v>15</v>
+        <f t="shared" si="3"/>
+        <v>12</v>
       </c>
       <c r="F31" s="2">
         <v>45181</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H31" t="s">
         <v>69</v>
@@ -1802,26 +1820,26 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>88</v>
+        <v>148</v>
       </c>
       <c r="B32">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C32" t="s">
         <v>10</v>
       </c>
       <c r="D32" s="4">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="E32" s="4">
-        <f t="shared" si="3"/>
-        <v>6</v>
+        <f t="shared" ref="E32:E33" si="4">PRODUCT(B32*D32)</f>
+        <v>15</v>
       </c>
       <c r="F32" s="2">
         <v>45181</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="H32" t="s">
         <v>69</v>
@@ -1829,10 +1847,10 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B33">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C33" t="s">
         <v>10</v>
@@ -1841,14 +1859,14 @@
         <v>3</v>
       </c>
       <c r="E33" s="4">
-        <f>PRODUCT(B33*D33)</f>
-        <v>12</v>
+        <f t="shared" si="4"/>
+        <v>6</v>
       </c>
       <c r="F33" s="2">
         <v>45181</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H33" t="s">
         <v>69</v>
@@ -1856,26 +1874,26 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
       <c r="B34">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C34" t="s">
         <v>10</v>
       </c>
       <c r="D34" s="4">
-        <v>22.9</v>
+        <v>3</v>
       </c>
       <c r="E34" s="4">
         <f>PRODUCT(B34*D34)</f>
-        <v>22.9</v>
+        <v>12</v>
       </c>
       <c r="F34" s="2">
         <v>45181</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H34" t="s">
         <v>69</v>
@@ -1883,34 +1901,34 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="B35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C35" t="s">
         <v>10</v>
       </c>
       <c r="D35" s="4">
-        <v>1.3</v>
+        <v>22.9</v>
       </c>
       <c r="E35" s="4">
-        <f t="shared" ref="E35:E41" si="4">PRODUCT(B35*D35)</f>
-        <v>2.6</v>
+        <f>PRODUCT(B35*D35)</f>
+        <v>22.9</v>
       </c>
       <c r="F35" s="2">
-        <v>45218</v>
+        <v>45181</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="H35" t="s">
-        <v>28</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B36">
         <v>2</v>
@@ -1919,17 +1937,17 @@
         <v>10</v>
       </c>
       <c r="D36" s="4">
-        <v>2</v>
+        <v>1.3</v>
       </c>
       <c r="E36" s="4">
-        <f t="shared" si="4"/>
-        <v>4</v>
+        <f t="shared" ref="E36:E42" si="5">PRODUCT(B36*D36)</f>
+        <v>2.6</v>
       </c>
       <c r="F36" s="2">
         <v>45218</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H36" t="s">
         <v>28</v>
@@ -1937,26 +1955,26 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>149</v>
+        <v>91</v>
       </c>
       <c r="B37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C37" t="s">
         <v>10</v>
       </c>
       <c r="D37" s="4">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="E37" s="4">
-        <f t="shared" si="4"/>
-        <v>25</v>
+        <f t="shared" si="5"/>
+        <v>4</v>
       </c>
       <c r="F37" s="2">
         <v>45218</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H37" t="s">
         <v>28</v>
@@ -1964,7 +1982,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -1973,17 +1991,17 @@
         <v>10</v>
       </c>
       <c r="D38" s="4">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E38" s="4">
-        <f t="shared" si="4"/>
-        <v>31</v>
+        <f t="shared" si="5"/>
+        <v>25</v>
       </c>
       <c r="F38" s="2">
         <v>45218</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H38" t="s">
         <v>28</v>
@@ -1991,34 +2009,34 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>92</v>
+        <v>150</v>
       </c>
       <c r="B39">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C39" t="s">
         <v>10</v>
       </c>
       <c r="D39" s="4">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="E39" s="4">
-        <f t="shared" si="4"/>
-        <v>8</v>
+        <f t="shared" si="5"/>
+        <v>31</v>
       </c>
       <c r="F39" s="2">
         <v>45218</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H39" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B40">
         <v>4</v>
@@ -2027,17 +2045,17 @@
         <v>10</v>
       </c>
       <c r="D40" s="4">
-        <v>1.7</v>
+        <v>2</v>
       </c>
       <c r="E40" s="4">
-        <f t="shared" si="4"/>
-        <v>6.8</v>
+        <f t="shared" si="5"/>
+        <v>8</v>
       </c>
       <c r="F40" s="2">
         <v>45218</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H40" t="s">
         <v>41</v>
@@ -2045,7 +2063,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>53</v>
+        <v>93</v>
       </c>
       <c r="B41">
         <v>4</v>
@@ -2054,52 +2072,52 @@
         <v>10</v>
       </c>
       <c r="D41" s="4">
-        <v>17.57</v>
+        <v>1.7</v>
       </c>
       <c r="E41" s="4">
-        <f t="shared" si="4"/>
-        <v>70.28</v>
+        <f t="shared" si="5"/>
+        <v>6.8</v>
       </c>
       <c r="F41" s="2">
-        <v>45257</v>
+        <v>45218</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>51</v>
+        <v>87</v>
       </c>
       <c r="H41" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>94</v>
+        <v>53</v>
       </c>
       <c r="B42">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C42" t="s">
         <v>10</v>
       </c>
       <c r="D42" s="4">
-        <v>44.75</v>
+        <v>17.57</v>
       </c>
       <c r="E42" s="4">
-        <f>PRODUCT(B42*D42)</f>
-        <v>44.75</v>
+        <f t="shared" si="5"/>
+        <v>70.28</v>
       </c>
       <c r="F42" s="2">
-        <v>45261</v>
+        <v>45257</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>95</v>
+        <v>51</v>
       </c>
       <c r="H42" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B43">
         <v>1</v>
@@ -2108,44 +2126,44 @@
         <v>10</v>
       </c>
       <c r="D43" s="4">
-        <v>1.85</v>
+        <v>44.75</v>
       </c>
       <c r="E43" s="4">
-        <f t="shared" ref="E43:E51" si="5">PRODUCT(B43*D43)</f>
-        <v>1.85</v>
+        <f>PRODUCT(B43*D43)</f>
+        <v>44.75</v>
       </c>
       <c r="F43" s="2">
-        <v>45267</v>
+        <v>45261</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H43" t="s">
-        <v>97</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>151</v>
+        <v>96</v>
       </c>
       <c r="B44">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="C44" t="s">
         <v>10</v>
       </c>
       <c r="D44" s="4">
-        <v>0.6</v>
+        <v>1.85</v>
       </c>
       <c r="E44" s="4">
-        <f t="shared" si="5"/>
-        <v>18</v>
+        <f t="shared" ref="E44:E52" si="6">PRODUCT(B44*D44)</f>
+        <v>1.85</v>
       </c>
       <c r="F44" s="2">
-        <v>45268</v>
+        <v>45267</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H44" t="s">
         <v>97</v>
@@ -2153,26 +2171,26 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>100</v>
+        <v>151</v>
       </c>
       <c r="B45">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="C45" t="s">
         <v>10</v>
       </c>
       <c r="D45" s="4">
-        <v>1.85</v>
+        <v>0.6</v>
       </c>
       <c r="E45" s="4">
-        <f t="shared" si="5"/>
-        <v>1.85</v>
+        <f t="shared" si="6"/>
+        <v>18</v>
       </c>
       <c r="F45" s="2">
         <v>45268</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="H45" t="s">
         <v>97</v>
@@ -2180,7 +2198,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -2189,17 +2207,17 @@
         <v>10</v>
       </c>
       <c r="D46" s="4">
-        <v>2</v>
+        <v>1.85</v>
       </c>
       <c r="E46" s="4">
-        <f t="shared" si="5"/>
-        <v>2</v>
+        <f t="shared" si="6"/>
+        <v>1.85</v>
       </c>
       <c r="F46" s="2">
         <v>45268</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H46" t="s">
         <v>97</v>
@@ -2207,7 +2225,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B47">
         <v>1</v>
@@ -2219,14 +2237,14 @@
         <v>2</v>
       </c>
       <c r="E47" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="F47" s="2">
         <v>45268</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="H47" t="s">
         <v>97</v>
@@ -2234,7 +2252,7 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B48">
         <v>1</v>
@@ -2246,14 +2264,14 @@
         <v>2</v>
       </c>
       <c r="E48" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="F48" s="2">
         <v>45268</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H48" t="s">
         <v>97</v>
@@ -2261,7 +2279,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B49">
         <v>1</v>
@@ -2273,14 +2291,14 @@
         <v>2</v>
       </c>
       <c r="E49" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="F49" s="2">
         <v>45268</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H49" t="s">
         <v>97</v>
@@ -2288,7 +2306,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B50">
         <v>1</v>
@@ -2300,14 +2318,14 @@
         <v>2</v>
       </c>
       <c r="E50" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="F50" s="2">
         <v>45268</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H50" t="s">
         <v>97</v>
@@ -2315,7 +2333,7 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B51">
         <v>1</v>
@@ -2324,17 +2342,17 @@
         <v>10</v>
       </c>
       <c r="D51" s="4">
-        <v>2.0499999999999998</v>
+        <v>2</v>
       </c>
       <c r="E51" s="4">
-        <f t="shared" si="5"/>
-        <v>2.0499999999999998</v>
+        <f t="shared" si="6"/>
+        <v>2</v>
       </c>
       <c r="F51" s="2">
         <v>45268</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H51" t="s">
         <v>97</v>
@@ -2342,26 +2360,26 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>152</v>
+        <v>108</v>
       </c>
       <c r="B52">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C52" t="s">
         <v>10</v>
       </c>
       <c r="D52" s="4">
-        <v>1.55</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="E52" s="4">
-        <f t="shared" ref="E52:E60" si="6">PRODUCT(B52*D52)</f>
-        <v>3.1</v>
+        <f t="shared" si="6"/>
+        <v>2.0499999999999998</v>
       </c>
       <c r="F52" s="2">
         <v>45268</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H52" t="s">
         <v>97</v>
@@ -2369,26 +2387,26 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B53">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C53" t="s">
         <v>10</v>
       </c>
       <c r="D53" s="4">
-        <v>2</v>
+        <v>1.55</v>
       </c>
       <c r="E53" s="4">
-        <f t="shared" si="6"/>
-        <v>2</v>
+        <f t="shared" ref="E53:E61" si="7">PRODUCT(B53*D53)</f>
+        <v>3.1</v>
       </c>
       <c r="F53" s="2">
         <v>45268</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H53" t="s">
         <v>97</v>
@@ -2396,7 +2414,7 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B54">
         <v>1</v>
@@ -2405,17 +2423,17 @@
         <v>10</v>
       </c>
       <c r="D54" s="4">
-        <v>1.95</v>
+        <v>2</v>
       </c>
       <c r="E54" s="4">
-        <f t="shared" si="6"/>
-        <v>1.95</v>
+        <f t="shared" si="7"/>
+        <v>2</v>
       </c>
       <c r="F54" s="2">
         <v>45268</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H54" t="s">
         <v>97</v>
@@ -2423,26 +2441,26 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>117</v>
+        <v>154</v>
       </c>
       <c r="B55">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C55" t="s">
         <v>10</v>
       </c>
       <c r="D55" s="4">
-        <v>2</v>
+        <v>1.95</v>
       </c>
       <c r="E55" s="4">
-        <f t="shared" si="6"/>
-        <v>4</v>
+        <f t="shared" si="7"/>
+        <v>1.95</v>
       </c>
       <c r="F55" s="2">
         <v>45268</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H55" t="s">
         <v>97</v>
@@ -2450,26 +2468,26 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C56" t="s">
         <v>10</v>
       </c>
       <c r="D56" s="4">
-        <v>2.65</v>
+        <v>2</v>
       </c>
       <c r="E56" s="4">
-        <f t="shared" si="6"/>
-        <v>2.65</v>
+        <f t="shared" si="7"/>
+        <v>4</v>
       </c>
       <c r="F56" s="2">
         <v>45268</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H56" t="s">
         <v>97</v>
@@ -2477,7 +2495,7 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B57">
         <v>1</v>
@@ -2486,17 +2504,17 @@
         <v>10</v>
       </c>
       <c r="D57" s="4">
-        <v>1.4</v>
+        <v>2.65</v>
       </c>
       <c r="E57" s="4">
-        <f t="shared" si="6"/>
-        <v>1.4</v>
+        <f t="shared" si="7"/>
+        <v>2.65</v>
       </c>
       <c r="F57" s="2">
         <v>45268</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H57" t="s">
         <v>97</v>
@@ -2504,53 +2522,53 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B58">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C58" t="s">
         <v>10</v>
       </c>
       <c r="D58" s="4">
-        <v>6</v>
+        <v>1.4</v>
       </c>
       <c r="E58" s="4">
-        <f t="shared" si="6"/>
-        <v>12</v>
+        <f t="shared" si="7"/>
+        <v>1.4</v>
       </c>
       <c r="F58" s="2">
-        <v>45270</v>
+        <v>45268</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H58" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B59">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C59" t="s">
         <v>10</v>
       </c>
       <c r="D59" s="4">
-        <v>34.9</v>
+        <v>6</v>
       </c>
       <c r="E59" s="4">
-        <f t="shared" si="6"/>
-        <v>34.9</v>
+        <f t="shared" si="7"/>
+        <v>12</v>
       </c>
       <c r="F59" s="2">
         <v>45270</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H59" t="s">
         <v>124</v>
@@ -2558,7 +2576,7 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B60">
         <v>1</v>
@@ -2567,17 +2585,17 @@
         <v>10</v>
       </c>
       <c r="D60" s="4">
-        <v>7.4</v>
+        <v>34.9</v>
       </c>
       <c r="E60" s="4">
-        <f t="shared" si="6"/>
-        <v>7.4</v>
+        <f t="shared" si="7"/>
+        <v>34.9</v>
       </c>
       <c r="F60" s="2">
         <v>45270</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="H60" t="s">
         <v>124</v>
@@ -2585,7 +2603,7 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B61">
         <v>1</v>
@@ -2594,17 +2612,17 @@
         <v>10</v>
       </c>
       <c r="D61" s="4">
-        <v>1.9</v>
+        <v>7.4</v>
       </c>
       <c r="E61" s="4">
-        <f t="shared" ref="E61:E66" si="7">PRODUCT(B61*D61)</f>
-        <v>1.9</v>
+        <f t="shared" si="7"/>
+        <v>7.4</v>
       </c>
       <c r="F61" s="2">
         <v>45270</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H61" t="s">
         <v>124</v>
@@ -2612,7 +2630,7 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B62">
         <v>1</v>
@@ -2621,17 +2639,17 @@
         <v>10</v>
       </c>
       <c r="D62" s="4">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="E62" s="4">
-        <f t="shared" si="7"/>
-        <v>1.8</v>
+        <f t="shared" ref="E62:E67" si="8">PRODUCT(B62*D62)</f>
+        <v>1.9</v>
       </c>
       <c r="F62" s="2">
         <v>45270</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="H62" t="s">
         <v>124</v>
@@ -2639,7 +2657,7 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B63">
         <v>1</v>
@@ -2648,17 +2666,17 @@
         <v>10</v>
       </c>
       <c r="D63" s="4">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="E63" s="4">
-        <f t="shared" si="7"/>
-        <v>2</v>
+        <f t="shared" si="8"/>
+        <v>1.8</v>
       </c>
       <c r="F63" s="2">
         <v>45270</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H63" t="s">
         <v>124</v>
@@ -2666,7 +2684,7 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B64">
         <v>1</v>
@@ -2678,14 +2696,14 @@
         <v>2</v>
       </c>
       <c r="E64" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="F64" s="2">
         <v>45270</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H64" t="s">
         <v>124</v>
@@ -2693,7 +2711,7 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B65">
         <v>1</v>
@@ -2702,44 +2720,44 @@
         <v>10</v>
       </c>
       <c r="D65" s="4">
-        <v>6.8</v>
+        <v>2</v>
       </c>
       <c r="E65" s="4">
-        <f t="shared" si="7"/>
-        <v>6.8</v>
+        <f t="shared" si="8"/>
+        <v>2</v>
       </c>
       <c r="F65" s="2">
         <v>45270</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="H65" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B66">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C66" t="s">
         <v>10</v>
       </c>
       <c r="D66" s="4">
-        <v>6.14</v>
+        <v>6.8</v>
       </c>
       <c r="E66" s="4">
-        <f t="shared" si="7"/>
-        <v>24.56</v>
+        <f t="shared" si="8"/>
+        <v>6.8</v>
       </c>
       <c r="F66" s="2">
         <v>45270</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H66" t="s">
         <v>138</v>
@@ -2747,61 +2765,61 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B67">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C67" t="s">
         <v>10</v>
       </c>
       <c r="D67" s="4">
-        <v>9.6</v>
+        <v>6.14</v>
       </c>
       <c r="E67" s="4">
-        <f>PRODUCT(B67*D67)</f>
-        <v>9.6</v>
+        <f t="shared" si="8"/>
+        <v>24.56</v>
       </c>
       <c r="F67" s="2">
-        <v>45323</v>
+        <v>45270</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="H67" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="B68">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C68" t="s">
         <v>10</v>
       </c>
       <c r="D68" s="4">
-        <v>1.5</v>
+        <v>9.6</v>
       </c>
       <c r="E68" s="4">
-        <f t="shared" ref="E68:E73" si="8">PRODUCT(B68*D68)</f>
-        <v>7.5</v>
+        <f>PRODUCT(B68*D68)</f>
+        <v>9.6</v>
       </c>
       <c r="F68" s="2">
-        <v>45336</v>
+        <v>45323</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="H68" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B69">
         <v>5</v>
@@ -2813,14 +2831,14 @@
         <v>1.5</v>
       </c>
       <c r="E69" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="E69:E74" si="9">PRODUCT(B69*D69)</f>
         <v>7.5</v>
       </c>
       <c r="F69" s="2">
         <v>45336</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H69" t="s">
         <v>159</v>
@@ -2828,26 +2846,26 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B70">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C70" t="s">
         <v>10</v>
       </c>
       <c r="D70" s="4">
-        <v>11</v>
+        <v>1.5</v>
       </c>
       <c r="E70" s="4">
-        <f t="shared" si="8"/>
-        <v>11</v>
+        <f t="shared" si="9"/>
+        <v>7.5</v>
       </c>
       <c r="F70" s="2">
         <v>45336</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="H70" t="s">
         <v>159</v>
@@ -2855,7 +2873,7 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B71">
         <v>1</v>
@@ -2864,17 +2882,17 @@
         <v>10</v>
       </c>
       <c r="D71" s="4">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E71" s="4">
-        <f t="shared" si="8"/>
-        <v>13</v>
+        <f t="shared" si="9"/>
+        <v>11</v>
       </c>
       <c r="F71" s="2">
         <v>45336</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H71" t="s">
         <v>159</v>
@@ -2882,7 +2900,7 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B72">
         <v>1</v>
@@ -2891,50 +2909,105 @@
         <v>10</v>
       </c>
       <c r="D72" s="4">
-        <v>22.6</v>
+        <v>13</v>
       </c>
       <c r="E72" s="4">
-        <f t="shared" si="8"/>
-        <v>22.6</v>
+        <f t="shared" si="9"/>
+        <v>13</v>
       </c>
       <c r="F72" s="2">
         <v>45336</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H72" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B73">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C73" t="s">
         <v>10</v>
       </c>
       <c r="D73" s="4">
-        <v>4.2699999999999996</v>
+        <v>22.6</v>
       </c>
       <c r="E73" s="4">
-        <f t="shared" si="8"/>
-        <v>17.079999999999998</v>
+        <f t="shared" si="9"/>
+        <v>22.6</v>
       </c>
       <c r="F73" s="2">
         <v>45336</v>
       </c>
       <c r="G73" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="H73" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>166</v>
+      </c>
+      <c r="B74">
+        <v>4</v>
+      </c>
+      <c r="C74" t="s">
+        <v>10</v>
+      </c>
+      <c r="D74" s="4">
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="E74" s="4">
+        <f t="shared" si="9"/>
+        <v>17.079999999999998</v>
+      </c>
+      <c r="F74" s="2">
+        <v>45336</v>
+      </c>
+      <c r="G74" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="H73" t="s">
+      <c r="H74" t="s">
         <v>143</v>
       </c>
     </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>169</v>
+      </c>
+      <c r="B75">
+        <v>1</v>
+      </c>
+      <c r="C75" t="s">
+        <v>10</v>
+      </c>
+      <c r="D75" s="4">
+        <v>34.61</v>
+      </c>
+      <c r="E75" s="4">
+        <f>PRODUCT(B75*D75)</f>
+        <v>34.61</v>
+      </c>
+      <c r="F75" s="2">
+        <v>45344</v>
+      </c>
+      <c r="G75" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="H75" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" xr:uid="{B6B23744-47F8-4A44-8ACF-D03494924EB0}"/>
     <hyperlink ref="G3" r:id="rId2" xr:uid="{2D76C7F9-FF91-48FB-AB7C-60DC37EB0B9B}"/>
@@ -2960,59 +3033,60 @@
     <hyperlink ref="G25" r:id="rId22" xr:uid="{B1D75C8F-A40A-4979-83D0-22AE1D3F8523}"/>
     <hyperlink ref="G22" r:id="rId23" xr:uid="{AA8B21F2-024D-432B-A6BD-1952FBEE2FD0}"/>
     <hyperlink ref="G23" r:id="rId24" xr:uid="{B3AD5637-8980-4F57-92DF-1CCB701E0E55}"/>
-    <hyperlink ref="G29" r:id="rId25" xr:uid="{67BB4281-9CBC-4C8A-A415-FE4F099C87FF}"/>
-    <hyperlink ref="G28" r:id="rId26" xr:uid="{010A41F6-DAAF-4AED-B438-036B0FB0E4F0}"/>
-    <hyperlink ref="G27" r:id="rId27" xr:uid="{9661D116-3AAF-48B2-AD54-2056078D7301}"/>
-    <hyperlink ref="G26" r:id="rId28" xr:uid="{6CA3E8EC-E5BB-4D96-B61C-1EDE7EB2D1C3}"/>
-    <hyperlink ref="G30" r:id="rId29" xr:uid="{4332FC3A-A51B-4368-9AC0-483D98BF86D9}"/>
-    <hyperlink ref="G34" r:id="rId30" xr:uid="{8F2DF8F4-E847-4DB0-B975-7C8914A7D0E1}"/>
-    <hyperlink ref="G32" r:id="rId31" xr:uid="{13ECFFB7-5315-4247-983C-5C2687A809CA}"/>
-    <hyperlink ref="G33" r:id="rId32" xr:uid="{84B4B117-EA41-4CDE-B53A-0BAA26B06B03}"/>
-    <hyperlink ref="G31" r:id="rId33" xr:uid="{68BD9474-984F-454C-9E53-DDDA097AB678}"/>
-    <hyperlink ref="G35" r:id="rId34" xr:uid="{B0079B2A-291D-42CB-A4B6-533D19DF527C}"/>
-    <hyperlink ref="G36" r:id="rId35" xr:uid="{960F0B4B-A8B2-4C2E-91B1-7DABB95476D2}"/>
-    <hyperlink ref="G37" r:id="rId36" xr:uid="{3B25B34F-C4C8-4D3E-A2CD-3490E409EA1A}"/>
-    <hyperlink ref="G38" r:id="rId37" xr:uid="{843B5765-13EC-4818-964E-DCE8554A4982}"/>
-    <hyperlink ref="G39" r:id="rId38" xr:uid="{EEACEC80-66C3-4FA5-9433-DF4C32F77567}"/>
-    <hyperlink ref="G40" r:id="rId39" xr:uid="{DD9DA7C6-B2EB-460F-98E3-14CF452D4609}"/>
-    <hyperlink ref="G41" r:id="rId40" xr:uid="{8D6E8713-2359-4426-BBB9-A1B7FB073886}"/>
-    <hyperlink ref="G42" r:id="rId41" xr:uid="{C0F43067-B0F6-4A19-80FD-3844EDBD59D5}"/>
-    <hyperlink ref="G43" r:id="rId42" xr:uid="{B7B248BF-2658-4CD3-870D-443C7E20C1D1}"/>
-    <hyperlink ref="G44" r:id="rId43" xr:uid="{02A43F30-3248-41EC-919F-8E2DF9EF4C90}"/>
-    <hyperlink ref="G45" r:id="rId44" xr:uid="{6C5C1868-DBBF-4D39-ADC7-B6DF17639981}"/>
-    <hyperlink ref="G46" r:id="rId45" xr:uid="{73FBFF06-BB90-44E6-9553-4007CE26D34A}"/>
-    <hyperlink ref="G47" r:id="rId46" xr:uid="{E0EDB21F-42E3-4758-A3EA-32A38D401B44}"/>
-    <hyperlink ref="G48" r:id="rId47" xr:uid="{F1C00F09-3511-4FDA-9AE3-51262AB18DD9}"/>
-    <hyperlink ref="G49" r:id="rId48" xr:uid="{5124D3AE-4AE7-4547-9F55-23DDAAC293E0}"/>
-    <hyperlink ref="G50" r:id="rId49" xr:uid="{204B228D-1027-4D52-8CC9-53BEF1F92201}"/>
-    <hyperlink ref="G51" r:id="rId50" xr:uid="{BBF830F1-9BDD-4AC2-B3AE-B7ADF515B8B1}"/>
-    <hyperlink ref="G52" r:id="rId51" xr:uid="{24C4D44B-21A8-4291-AAEC-224B562F813D}"/>
-    <hyperlink ref="G53" r:id="rId52" xr:uid="{EFD84485-999F-4DB4-B6C7-71A856C5BCB7}"/>
-    <hyperlink ref="G54" r:id="rId53" xr:uid="{A539AFAC-7041-4BC0-8DC8-88766104432E}"/>
-    <hyperlink ref="G55" r:id="rId54" xr:uid="{F335BDA5-520A-45DE-B4EA-BEA5B13B7404}"/>
-    <hyperlink ref="G56" r:id="rId55" xr:uid="{AAF15848-E84A-4100-BCE5-EDA9A8E25CD6}"/>
-    <hyperlink ref="G57" r:id="rId56" xr:uid="{D1C61C6A-4337-46EA-9E44-9A85AB56ED64}"/>
-    <hyperlink ref="G58" r:id="rId57" xr:uid="{AEA52DF4-3B50-4A0A-8D94-D64E4E81CE28}"/>
-    <hyperlink ref="G59" r:id="rId58" xr:uid="{55A53144-E181-40EE-9960-D1B79387DFC4}"/>
-    <hyperlink ref="G60" r:id="rId59" xr:uid="{7A64D824-FBFC-4ED4-B850-1A9E2113026B}"/>
-    <hyperlink ref="G61" r:id="rId60" xr:uid="{54C0B32C-ADE3-43D1-878A-283B1B230D41}"/>
-    <hyperlink ref="G62" r:id="rId61" xr:uid="{A424218F-5661-478F-9084-FC177CE4FFAF}"/>
-    <hyperlink ref="G63" r:id="rId62" xr:uid="{90BAC5E7-03D4-44E9-BFDA-CB6B6DCA44C9}"/>
-    <hyperlink ref="G64" r:id="rId63" xr:uid="{2406F597-5C18-4115-8005-0E9BB3DE6E31}"/>
-    <hyperlink ref="G66" r:id="rId64" xr:uid="{CCC2B9B3-CDEB-45B6-BDFE-47325C9B448B}"/>
-    <hyperlink ref="G65" r:id="rId65" xr:uid="{1C79B802-BE99-4678-804D-C270068D64CA}"/>
-    <hyperlink ref="G67" r:id="rId66" xr:uid="{72DA93FE-CFC2-4B24-B87A-ACF218C75DDB}"/>
-    <hyperlink ref="G69" r:id="rId67" xr:uid="{98B2BF96-CECA-4997-8F9A-6C7FBB70FD0F}"/>
-    <hyperlink ref="G68" r:id="rId68" xr:uid="{0DC58D63-9AAC-4788-8030-06CE5D99938A}"/>
-    <hyperlink ref="G70" r:id="rId69" xr:uid="{7225F3AF-B472-487F-B13C-85484FF39D7A}"/>
-    <hyperlink ref="G71" r:id="rId70" xr:uid="{5EDD8DBB-DBAD-47D9-8767-118A0E0E872A}"/>
-    <hyperlink ref="G72" r:id="rId71" xr:uid="{FC2C26D6-0C48-4854-908D-8D944232D4DF}"/>
-    <hyperlink ref="G73" r:id="rId72" xr:uid="{6215BBD2-B0C6-449F-8D2F-97AC4456E538}"/>
+    <hyperlink ref="G30" r:id="rId25" xr:uid="{67BB4281-9CBC-4C8A-A415-FE4F099C87FF}"/>
+    <hyperlink ref="G29" r:id="rId26" xr:uid="{010A41F6-DAAF-4AED-B438-036B0FB0E4F0}"/>
+    <hyperlink ref="G28" r:id="rId27" xr:uid="{9661D116-3AAF-48B2-AD54-2056078D7301}"/>
+    <hyperlink ref="G27" r:id="rId28" xr:uid="{6CA3E8EC-E5BB-4D96-B61C-1EDE7EB2D1C3}"/>
+    <hyperlink ref="G31" r:id="rId29" xr:uid="{4332FC3A-A51B-4368-9AC0-483D98BF86D9}"/>
+    <hyperlink ref="G35" r:id="rId30" xr:uid="{8F2DF8F4-E847-4DB0-B975-7C8914A7D0E1}"/>
+    <hyperlink ref="G33" r:id="rId31" xr:uid="{13ECFFB7-5315-4247-983C-5C2687A809CA}"/>
+    <hyperlink ref="G34" r:id="rId32" xr:uid="{84B4B117-EA41-4CDE-B53A-0BAA26B06B03}"/>
+    <hyperlink ref="G32" r:id="rId33" xr:uid="{68BD9474-984F-454C-9E53-DDDA097AB678}"/>
+    <hyperlink ref="G36" r:id="rId34" xr:uid="{B0079B2A-291D-42CB-A4B6-533D19DF527C}"/>
+    <hyperlink ref="G37" r:id="rId35" xr:uid="{960F0B4B-A8B2-4C2E-91B1-7DABB95476D2}"/>
+    <hyperlink ref="G38" r:id="rId36" xr:uid="{3B25B34F-C4C8-4D3E-A2CD-3490E409EA1A}"/>
+    <hyperlink ref="G39" r:id="rId37" xr:uid="{843B5765-13EC-4818-964E-DCE8554A4982}"/>
+    <hyperlink ref="G40" r:id="rId38" xr:uid="{EEACEC80-66C3-4FA5-9433-DF4C32F77567}"/>
+    <hyperlink ref="G41" r:id="rId39" xr:uid="{DD9DA7C6-B2EB-460F-98E3-14CF452D4609}"/>
+    <hyperlink ref="G42" r:id="rId40" xr:uid="{8D6E8713-2359-4426-BBB9-A1B7FB073886}"/>
+    <hyperlink ref="G43" r:id="rId41" xr:uid="{C0F43067-B0F6-4A19-80FD-3844EDBD59D5}"/>
+    <hyperlink ref="G44" r:id="rId42" xr:uid="{B7B248BF-2658-4CD3-870D-443C7E20C1D1}"/>
+    <hyperlink ref="G45" r:id="rId43" xr:uid="{02A43F30-3248-41EC-919F-8E2DF9EF4C90}"/>
+    <hyperlink ref="G46" r:id="rId44" xr:uid="{6C5C1868-DBBF-4D39-ADC7-B6DF17639981}"/>
+    <hyperlink ref="G47" r:id="rId45" xr:uid="{73FBFF06-BB90-44E6-9553-4007CE26D34A}"/>
+    <hyperlink ref="G48" r:id="rId46" xr:uid="{E0EDB21F-42E3-4758-A3EA-32A38D401B44}"/>
+    <hyperlink ref="G49" r:id="rId47" xr:uid="{F1C00F09-3511-4FDA-9AE3-51262AB18DD9}"/>
+    <hyperlink ref="G50" r:id="rId48" xr:uid="{5124D3AE-4AE7-4547-9F55-23DDAAC293E0}"/>
+    <hyperlink ref="G51" r:id="rId49" xr:uid="{204B228D-1027-4D52-8CC9-53BEF1F92201}"/>
+    <hyperlink ref="G52" r:id="rId50" xr:uid="{BBF830F1-9BDD-4AC2-B3AE-B7ADF515B8B1}"/>
+    <hyperlink ref="G53" r:id="rId51" xr:uid="{24C4D44B-21A8-4291-AAEC-224B562F813D}"/>
+    <hyperlink ref="G54" r:id="rId52" xr:uid="{EFD84485-999F-4DB4-B6C7-71A856C5BCB7}"/>
+    <hyperlink ref="G55" r:id="rId53" xr:uid="{A539AFAC-7041-4BC0-8DC8-88766104432E}"/>
+    <hyperlink ref="G56" r:id="rId54" xr:uid="{F335BDA5-520A-45DE-B4EA-BEA5B13B7404}"/>
+    <hyperlink ref="G57" r:id="rId55" xr:uid="{AAF15848-E84A-4100-BCE5-EDA9A8E25CD6}"/>
+    <hyperlink ref="G58" r:id="rId56" xr:uid="{D1C61C6A-4337-46EA-9E44-9A85AB56ED64}"/>
+    <hyperlink ref="G59" r:id="rId57" xr:uid="{AEA52DF4-3B50-4A0A-8D94-D64E4E81CE28}"/>
+    <hyperlink ref="G60" r:id="rId58" xr:uid="{55A53144-E181-40EE-9960-D1B79387DFC4}"/>
+    <hyperlink ref="G61" r:id="rId59" xr:uid="{7A64D824-FBFC-4ED4-B850-1A9E2113026B}"/>
+    <hyperlink ref="G62" r:id="rId60" xr:uid="{54C0B32C-ADE3-43D1-878A-283B1B230D41}"/>
+    <hyperlink ref="G63" r:id="rId61" xr:uid="{A424218F-5661-478F-9084-FC177CE4FFAF}"/>
+    <hyperlink ref="G64" r:id="rId62" xr:uid="{90BAC5E7-03D4-44E9-BFDA-CB6B6DCA44C9}"/>
+    <hyperlink ref="G65" r:id="rId63" xr:uid="{2406F597-5C18-4115-8005-0E9BB3DE6E31}"/>
+    <hyperlink ref="G67" r:id="rId64" xr:uid="{CCC2B9B3-CDEB-45B6-BDFE-47325C9B448B}"/>
+    <hyperlink ref="G66" r:id="rId65" xr:uid="{1C79B802-BE99-4678-804D-C270068D64CA}"/>
+    <hyperlink ref="G68" r:id="rId66" xr:uid="{72DA93FE-CFC2-4B24-B87A-ACF218C75DDB}"/>
+    <hyperlink ref="G70" r:id="rId67" xr:uid="{98B2BF96-CECA-4997-8F9A-6C7FBB70FD0F}"/>
+    <hyperlink ref="G69" r:id="rId68" xr:uid="{0DC58D63-9AAC-4788-8030-06CE5D99938A}"/>
+    <hyperlink ref="G71" r:id="rId69" xr:uid="{7225F3AF-B472-487F-B13C-85484FF39D7A}"/>
+    <hyperlink ref="G72" r:id="rId70" xr:uid="{5EDD8DBB-DBAD-47D9-8767-118A0E0E872A}"/>
+    <hyperlink ref="G73" r:id="rId71" xr:uid="{FC2C26D6-0C48-4854-908D-8D944232D4DF}"/>
+    <hyperlink ref="G74" r:id="rId72" xr:uid="{6215BBD2-B0C6-449F-8D2F-97AC4456E538}"/>
+    <hyperlink ref="G75" r:id="rId73" xr:uid="{5D290A41-911B-46BB-B5F5-0B1CA2DBCF83}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">
-    <tablePart r:id="rId73"/>
     <tablePart r:id="rId74"/>
+    <tablePart r:id="rId75"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>